<commit_message>
Error in nested property
</commit_message>
<xml_diff>
--- a/Tests/TestImporData.xlsx
+++ b/Tests/TestImporData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joche\source\repos\XafImportApiWithTest\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8F699B-9E7C-4652-8529-9CC70FC689E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDBFE4A-8B1A-4CDE-87F0-26F7E32D5FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{142291C4-3925-4944-A539-5D3AA6751861}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{142291C4-3925-4944-A539-5D3AA6751861}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29510,15 +29510,15 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>